<commit_message>
Updated files relevant to work on RXC J2211.
Still have a few more bands that could be reduced.
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="2500" windowWidth="22280" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="2000" yWindow="6160" windowWidth="26860" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RELICS Sample" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="653">
   <si>
     <t>Semester</t>
   </si>
@@ -1981,10 +1981,10 @@
     <t>?</t>
   </si>
   <si>
-    <t>wd* (need to rename jvo flats)</t>
-  </si>
-  <si>
-    <t>wd* (SMOKA query made, need to download)</t>
+    <t>~0.4-1" seeing; image doesn't look great in the northeast corner (center looks OK).</t>
+  </si>
+  <si>
+    <t>Missing some chips; looks OK but uneven field, likely due to missing chip</t>
   </si>
 </sst>
 </file>
@@ -3094,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="L136" sqref="L136"/>
+    <sheetView tabSelected="1" topLeftCell="C111" workbookViewId="0">
+      <selection activeCell="N131" sqref="N131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9136,12 +9136,16 @@
       <c r="M128" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N128" s="10"/>
-      <c r="O128" s="10"/>
+      <c r="N128" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O128" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="P128" s="10"/>
       <c r="Q128" s="10"/>
       <c r="R128" s="10" t="s">
-        <v>461</v>
+        <v>652</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.2">
@@ -9230,12 +9234,16 @@
       <c r="M130" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N130" s="10"/>
-      <c r="O130" s="10"/>
+      <c r="N130" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O130" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="P130" s="10"/>
       <c r="Q130" s="10"/>
       <c r="R130" s="10" t="s">
-        <v>479</v>
+        <v>651</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.2">
@@ -9320,10 +9328,14 @@
       </c>
       <c r="L132" s="10"/>
       <c r="M132" s="10" t="s">
-        <v>651</v>
-      </c>
-      <c r="N132" s="10"/>
-      <c r="O132" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="N132" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O132" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="P132" s="10"/>
       <c r="Q132" s="10"/>
       <c r="R132" s="10" t="s">
@@ -9418,8 +9430,12 @@
       <c r="M134" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N134" s="10"/>
-      <c r="O134" s="10"/>
+      <c r="N134" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O134" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="P134" s="10"/>
       <c r="Q134" s="10"/>
       <c r="R134" s="10" t="s">
@@ -9461,11 +9477,17 @@
         <v>36</v>
       </c>
       <c r="L135" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="M135" s="10"/>
-      <c r="N135" s="10"/>
-      <c r="O135" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="M135" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N135" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O135" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="P135" s="10"/>
       <c r="Q135" s="10" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Updated reduction status list to reflect work on A1763.
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawson/Git/RELICSSuprimeCam/Reduction Notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawson29/Git/RELICSSuprimeCam/Reduction Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="6160" windowWidth="26860" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="9800" windowWidth="26860" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RELICS Sample" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,8 +28,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="O33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>wd:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+This data wasn't very good, probably due to the thich cirrus and relatively short exposure time. So I didn't include it in the reduction stack.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="654">
   <si>
     <t>Semester</t>
   </si>
@@ -1985,6 +2021,9 @@
   </si>
   <si>
     <t>Missing some chips; looks OK but uneven field, likely due to missing chip</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2033,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mmm\-dd;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2136,6 +2175,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2228,7 +2278,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2337,6 +2387,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2378,12 +2429,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mmm\-dd;@"/>
     </dxf>
@@ -2730,6 +2775,12 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -2755,9 +2806,9 @@
     <tableColumn id="5" name="Raw Data"/>
     <tableColumn id="6" name="FRAMEID_start"/>
     <tableColumn id="7" name="FRAMID_end"/>
-    <tableColumn id="8" name="Exposures" dataDxfId="1"/>
+    <tableColumn id="8" name="Exposures" dataDxfId="22"/>
     <tableColumn id="9" name="Exposure (s)"/>
-    <tableColumn id="10" name="Total Exp (m)" dataDxfId="0"/>
+    <tableColumn id="10" name="Total Exp (m)" dataDxfId="21"/>
     <tableColumn id="11" name="Flat Raw"/>
     <tableColumn id="12" name="Flat Reduced"/>
     <tableColumn id="13" name="Image"/>
@@ -2771,44 +2822,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q85" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q85" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:Q85"/>
   <sortState ref="A2:Q54">
     <sortCondition ref="A1:A54"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Cluster" dataDxfId="20"/>
-    <tableColumn id="2" name="Date" dataDxfId="19"/>
-    <tableColumn id="3" name="Semester" dataDxfId="18"/>
-    <tableColumn id="4" name="Band" dataDxfId="17"/>
-    <tableColumn id="5" name="Raw Data" dataDxfId="16"/>
-    <tableColumn id="6" name="FRAMEID_start" dataDxfId="15"/>
-    <tableColumn id="7" name="FRAMID_end" dataDxfId="14"/>
-    <tableColumn id="8" name="Exposures" dataDxfId="13">
+    <tableColumn id="1" name="Cluster" dataDxfId="18"/>
+    <tableColumn id="2" name="Date" dataDxfId="17"/>
+    <tableColumn id="3" name="Semester" dataDxfId="16"/>
+    <tableColumn id="4" name="Band" dataDxfId="15"/>
+    <tableColumn id="5" name="Raw Data" dataDxfId="14"/>
+    <tableColumn id="6" name="FRAMEID_start" dataDxfId="13"/>
+    <tableColumn id="7" name="FRAMID_end" dataDxfId="12"/>
+    <tableColumn id="8" name="Exposures" dataDxfId="11">
       <calculatedColumnFormula>(RIGHT(G2,LEN(G2)-4)-RIGHT(F2,LEN(F2)-4)+1)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Exposure (s)" dataDxfId="12"/>
-    <tableColumn id="10" name="Total Exp (m)" dataDxfId="11">
+    <tableColumn id="9" name="Exposure (s)" dataDxfId="10"/>
+    <tableColumn id="10" name="Total Exp (m)" dataDxfId="9">
       <calculatedColumnFormula>H2*I2/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Flat Raw" dataDxfId="10"/>
-    <tableColumn id="12" name="Flat Reduced" dataDxfId="9"/>
-    <tableColumn id="13" name="Image" dataDxfId="8"/>
-    <tableColumn id="14" name="SExtractor Catalog" dataDxfId="7"/>
-    <tableColumn id="15" name="Shapes" dataDxfId="6"/>
-    <tableColumn id="16" name="Deep Band?" dataDxfId="5"/>
-    <tableColumn id="17" name="Comment" dataDxfId="4"/>
+    <tableColumn id="11" name="Flat Raw" dataDxfId="8"/>
+    <tableColumn id="12" name="Flat Reduced" dataDxfId="7"/>
+    <tableColumn id="13" name="Image" dataDxfId="6"/>
+    <tableColumn id="14" name="SExtractor Catalog" dataDxfId="5"/>
+    <tableColumn id="15" name="Shapes" dataDxfId="4"/>
+    <tableColumn id="16" name="Deep Band?" dataDxfId="3"/>
+    <tableColumn id="17" name="Comment" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q113" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q113" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:Q113"/>
   <tableColumns count="17">
     <tableColumn id="2" name="Cluster"/>
-    <tableColumn id="1" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="0"/>
     <tableColumn id="17" name="Semester2"/>
     <tableColumn id="3" name="Band"/>
     <tableColumn id="4" name="Raw Data"/>
@@ -3091,11 +3142,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C111" workbookViewId="0">
-      <selection activeCell="N131" sqref="N131"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4355,14 +4406,14 @@
         <v>560</v>
       </c>
       <c r="I19" s="10">
-        <f>(RIGHT(H19,LEN(H19)-4)-RIGHT(G19,LEN(G19)-4)+1)/10</f>
+        <f t="shared" ref="I19:I31" si="0">(RIGHT(H19,LEN(H19)-4)-RIGHT(G19,LEN(G19)-4)+1)/10</f>
         <v>4</v>
       </c>
       <c r="J19" s="10">
         <v>180</v>
       </c>
       <c r="K19" s="60">
-        <f>I19*J19/60</f>
+        <f t="shared" ref="K19:K31" si="1">I19*J19/60</f>
         <v>12</v>
       </c>
       <c r="L19" s="10"/>
@@ -4399,14 +4450,14 @@
         <v>562</v>
       </c>
       <c r="I20" s="10">
-        <f>(RIGHT(H20,LEN(H20)-4)-RIGHT(G20,LEN(G20)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J20" s="10">
         <v>360</v>
       </c>
       <c r="K20" s="60">
-        <f>I20*J20/60</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="L20" s="10"/>
@@ -4443,14 +4494,14 @@
         <v>564</v>
       </c>
       <c r="I21" s="10">
-        <f>(RIGHT(H21,LEN(H21)-4)-RIGHT(G21,LEN(G21)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="J21" s="10">
         <v>150</v>
       </c>
       <c r="K21" s="60">
-        <f>I21*J21/60</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="L21" s="10"/>
@@ -4487,14 +4538,14 @@
         <v>566</v>
       </c>
       <c r="I22" s="10">
-        <f>(RIGHT(H22,LEN(H22)-4)-RIGHT(G22,LEN(G22)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J22" s="10">
         <v>600</v>
       </c>
       <c r="K22" s="60">
-        <f>I22*J22/60</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="L22" s="10"/>
@@ -4531,14 +4582,14 @@
         <v>568</v>
       </c>
       <c r="I23" s="10">
-        <f>(RIGHT(H23,LEN(H23)-4)-RIGHT(G23,LEN(G23)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J23" s="10">
         <v>500</v>
       </c>
       <c r="K23" s="60">
-        <f>I23*J23/60</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="L23" s="10"/>
@@ -4577,14 +4628,14 @@
         <v>570</v>
       </c>
       <c r="I24" s="10">
-        <f>(RIGHT(H24,LEN(H24)-4)-RIGHT(G24,LEN(G24)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="J24" s="10">
         <v>600</v>
       </c>
       <c r="K24" s="60">
-        <f>I24*J24/60</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="L24" s="10"/>
@@ -4621,14 +4672,14 @@
         <v>572</v>
       </c>
       <c r="I25" s="10">
-        <f>(RIGHT(H25,LEN(H25)-4)-RIGHT(G25,LEN(G25)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J25" s="10">
         <v>500</v>
       </c>
       <c r="K25" s="60">
-        <f>I25*J25/60</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="L25" s="10"/>
@@ -4665,14 +4716,14 @@
         <v>574</v>
       </c>
       <c r="I26" s="10">
-        <f>(RIGHT(H26,LEN(H26)-4)-RIGHT(G26,LEN(G26)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J26" s="10">
         <v>600</v>
       </c>
       <c r="K26" s="60">
-        <f>I26*J26/60</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="L26" s="10"/>
@@ -4709,14 +4760,14 @@
         <v>576</v>
       </c>
       <c r="I27" s="10">
-        <f>(RIGHT(H27,LEN(H27)-4)-RIGHT(G27,LEN(G27)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J27" s="10">
         <v>120</v>
       </c>
       <c r="K27" s="60">
-        <f>I27*J27/60</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="L27" s="10"/>
@@ -4753,14 +4804,14 @@
         <v>578</v>
       </c>
       <c r="I28" s="10">
-        <f>(RIGHT(H28,LEN(H28)-4)-RIGHT(G28,LEN(G28)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J28" s="10">
         <v>300</v>
       </c>
       <c r="K28" s="60">
-        <f>I28*J28/60</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="L28" s="10"/>
@@ -4797,14 +4848,14 @@
         <v>580</v>
       </c>
       <c r="I29" s="10">
-        <f>(RIGHT(H29,LEN(H29)-4)-RIGHT(G29,LEN(G29)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="J29" s="10">
         <v>300</v>
       </c>
       <c r="K29" s="60">
-        <f>I29*J29/60</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="L29" s="10"/>
@@ -4841,14 +4892,14 @@
         <v>582</v>
       </c>
       <c r="I30" s="10">
-        <f>(RIGHT(H30,LEN(H30)-4)-RIGHT(G30,LEN(G30)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J30" s="10">
         <v>180</v>
       </c>
       <c r="K30" s="60">
-        <f>I30*J30/60</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="L30" s="10"/>
@@ -4885,14 +4936,14 @@
         <v>584</v>
       </c>
       <c r="I31" s="10">
-        <f>(RIGHT(H31,LEN(H31)-4)-RIGHT(G31,LEN(G31)-4)+1)/10</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="J31" s="10">
         <v>240</v>
       </c>
       <c r="K31" s="60">
-        <f>I31*J31/60</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="L31" s="10"/>
@@ -4949,21 +5000,17 @@
         <f>'MC3PO Sample'!J40</f>
         <v>8</v>
       </c>
-      <c r="L32" s="12">
-        <f>'MC3PO Sample'!K40</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="12">
-        <f>'MC3PO Sample'!L40</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="12">
-        <f>'MC3PO Sample'!M40</f>
-        <v>0</v>
-      </c>
-      <c r="O32" s="12">
-        <f>'MC3PO Sample'!N40</f>
-        <v>0</v>
+      <c r="L32" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="P32" s="12">
         <f>'MC3PO Sample'!O40</f>
@@ -5022,21 +5069,17 @@
         <f>'MC3PO Sample'!J41</f>
         <v>16</v>
       </c>
-      <c r="L33" s="12">
-        <f>'MC3PO Sample'!K41</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="12">
-        <f>'MC3PO Sample'!L41</f>
-        <v>0</v>
-      </c>
-      <c r="N33" s="12">
-        <f>'MC3PO Sample'!M41</f>
-        <v>0</v>
-      </c>
-      <c r="O33" s="12">
-        <f>'MC3PO Sample'!N41</f>
-        <v>0</v>
+      <c r="L33" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" s="108" t="s">
+        <v>653</v>
       </c>
       <c r="P33" s="12">
         <f>'MC3PO Sample'!O41</f>
@@ -5095,21 +5138,17 @@
         <f>'MC3PO Sample'!J42</f>
         <v>28</v>
       </c>
-      <c r="L34" s="12">
-        <f>'MC3PO Sample'!K42</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="12">
-        <f>'MC3PO Sample'!L42</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="12">
-        <f>'MC3PO Sample'!M42</f>
-        <v>0</v>
-      </c>
-      <c r="O34" s="12">
-        <f>'MC3PO Sample'!N42</f>
-        <v>0</v>
+      <c r="L34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="P34" s="12">
         <f>'MC3PO Sample'!O42</f>
@@ -5168,21 +5207,17 @@
         <f>'MC3PO Sample'!J43</f>
         <v>28</v>
       </c>
-      <c r="L35" s="12">
-        <f>'MC3PO Sample'!K43</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="12">
-        <f>'MC3PO Sample'!L43</f>
-        <v>0</v>
-      </c>
-      <c r="N35" s="12">
-        <f>'MC3PO Sample'!M43</f>
-        <v>0</v>
-      </c>
-      <c r="O35" s="12">
-        <f>'MC3PO Sample'!N43</f>
-        <v>0</v>
+      <c r="L35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="P35" s="12">
         <f>'MC3PO Sample'!O43</f>
@@ -5241,21 +5276,17 @@
         <f>'MC3PO Sample'!J44</f>
         <v>28</v>
       </c>
-      <c r="L36" s="12">
-        <f>'MC3PO Sample'!K44</f>
-        <v>0</v>
-      </c>
-      <c r="M36" s="12">
-        <f>'MC3PO Sample'!L44</f>
-        <v>0</v>
-      </c>
-      <c r="N36" s="12">
-        <f>'MC3PO Sample'!M44</f>
-        <v>0</v>
-      </c>
-      <c r="O36" s="12">
-        <f>'MC3PO Sample'!N44</f>
-        <v>0</v>
+      <c r="L36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="P36" s="12">
         <f>'MC3PO Sample'!O44</f>
@@ -5294,14 +5325,14 @@
         <v>226</v>
       </c>
       <c r="I37" s="4">
-        <f>(RIGHT(H37,LEN(H37)-4)-RIGHT(G37,LEN(G37)-4)+1)/10</f>
+        <f t="shared" ref="I37:I42" si="2">(RIGHT(H37,LEN(H37)-4)-RIGHT(G37,LEN(G37)-4)+1)/10</f>
         <v>15</v>
       </c>
       <c r="J37" s="4">
         <v>300</v>
       </c>
       <c r="K37" s="64">
-        <f>I37*J37/60</f>
+        <f t="shared" ref="K37:K42" si="3">I37*J37/60</f>
         <v>75</v>
       </c>
       <c r="L37" s="4"/>
@@ -5340,14 +5371,14 @@
         <v>228</v>
       </c>
       <c r="I38" s="4">
-        <f>(RIGHT(H38,LEN(H38)-4)-RIGHT(G38,LEN(G38)-4)+1)/10</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J38" s="4">
         <v>300</v>
       </c>
       <c r="K38" s="64">
-        <f>I38*J38/60</f>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="L38" s="4"/>
@@ -5384,14 +5415,14 @@
         <v>230</v>
       </c>
       <c r="I39" s="4">
-        <f>(RIGHT(H39,LEN(H39)-4)-RIGHT(G39,LEN(G39)-4)+1)/10</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J39" s="4">
         <v>300</v>
       </c>
       <c r="K39" s="64">
-        <f>I39*J39/60</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L39" s="4"/>
@@ -5428,14 +5459,14 @@
         <v>484</v>
       </c>
       <c r="I40" s="8">
-        <f>(RIGHT(H40,LEN(H40)-4)-RIGHT(G40,LEN(G40)-4)+1)/10</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J40" s="8">
         <v>480</v>
       </c>
       <c r="K40" s="66">
-        <f>I40*J40/60</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L40" s="8"/>
@@ -5474,14 +5505,14 @@
         <v>486</v>
       </c>
       <c r="I41" s="8">
-        <f>(RIGHT(H41,LEN(H41)-4)-RIGHT(G41,LEN(G41)-4)+1)/10</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J41" s="8">
         <v>240</v>
       </c>
       <c r="K41" s="66">
-        <f>I41*J41/60</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="L41" s="8"/>
@@ -5518,14 +5549,14 @@
         <v>488</v>
       </c>
       <c r="I42" s="8">
-        <f>(RIGHT(H42,LEN(H42)-4)-RIGHT(G42,LEN(G42)-4)+1)/10</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J42" s="8">
         <v>180</v>
       </c>
       <c r="K42" s="66">
-        <f>I42*J42/60</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="L42" s="8"/>
@@ -5859,14 +5890,14 @@
         <v>640</v>
       </c>
       <c r="I49" s="14">
-        <f>(RIGHT(H49,LEN(H49)-4)-RIGHT(G49,LEN(G49)-4)+1)/10</f>
+        <f t="shared" ref="I49:I65" si="4">(RIGHT(H49,LEN(H49)-4)-RIGHT(G49,LEN(G49)-4)+1)/10</f>
         <v>10</v>
       </c>
       <c r="J49" s="14">
         <v>720</v>
       </c>
       <c r="K49" s="95">
-        <f>I49*J49/60</f>
+        <f t="shared" ref="K49:K65" si="5">I49*J49/60</f>
         <v>120</v>
       </c>
       <c r="L49" s="14"/>
@@ -5905,14 +5936,14 @@
         <v>642</v>
       </c>
       <c r="I50" s="14">
-        <f>(RIGHT(H50,LEN(H50)-4)-RIGHT(G50,LEN(G50)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="J50" s="14">
         <v>300</v>
       </c>
       <c r="K50" s="95">
-        <f>I50*J50/60</f>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="L50" s="14"/>
@@ -5951,14 +5982,14 @@
         <v>644</v>
       </c>
       <c r="I51" s="14">
-        <f>(RIGHT(H51,LEN(H51)-4)-RIGHT(G51,LEN(G51)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="J51" s="14">
         <v>480</v>
       </c>
       <c r="K51" s="95">
-        <f>I51*J51/60</f>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
       <c r="L51" s="14"/>
@@ -5997,14 +6028,14 @@
         <v>646</v>
       </c>
       <c r="I52" s="14">
-        <f>(RIGHT(H52,LEN(H52)-4)-RIGHT(G52,LEN(G52)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="J52" s="14">
         <v>180</v>
       </c>
       <c r="K52" s="95">
-        <f>I52*J52/60</f>
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
       <c r="L52" s="14"/>
@@ -6041,14 +6072,14 @@
         <v>433</v>
       </c>
       <c r="I53" s="8">
-        <f>(RIGHT(H53,LEN(H53)-4)-RIGHT(G53,LEN(G53)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J53" s="8">
         <v>240</v>
       </c>
       <c r="K53" s="66">
-        <f>I53*J53/60</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L53" s="8"/>
@@ -6085,14 +6116,14 @@
         <v>435</v>
       </c>
       <c r="I54" s="8">
-        <f>(RIGHT(H54,LEN(H54)-4)-RIGHT(G54,LEN(G54)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J54" s="8">
         <v>240</v>
       </c>
       <c r="K54" s="66">
-        <f>I54*J54/60</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L54" s="8"/>
@@ -6129,14 +6160,14 @@
         <v>437</v>
       </c>
       <c r="I55" s="8">
-        <f>(RIGHT(H55,LEN(H55)-4)-RIGHT(G55,LEN(G55)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="J55" s="8">
         <v>240</v>
       </c>
       <c r="K55" s="66">
-        <f>I55*J55/60</f>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L55" s="8"/>
@@ -6175,14 +6206,14 @@
         <v>439</v>
       </c>
       <c r="I56" s="8">
-        <f>(RIGHT(H56,LEN(H56)-4)-RIGHT(G56,LEN(G56)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="J56" s="8">
         <v>180</v>
       </c>
       <c r="K56" s="66">
-        <f>I56*J56/60</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="L56" s="8"/>
@@ -6219,14 +6250,14 @@
         <v>441</v>
       </c>
       <c r="I57" s="8">
-        <f>(RIGHT(H57,LEN(H57)-4)-RIGHT(G57,LEN(G57)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="J57" s="8">
         <v>180</v>
       </c>
       <c r="K57" s="66">
-        <f>I57*J57/60</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="L57" s="8"/>
@@ -6263,14 +6294,14 @@
         <v>624</v>
       </c>
       <c r="I58" s="12">
-        <f>(RIGHT(H58,LEN(H58)-4)-RIGHT(G58,LEN(G58)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J58" s="12">
         <v>480</v>
       </c>
       <c r="K58" s="91">
-        <f>I58*J58/60</f>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L58" s="12"/>
@@ -6309,14 +6340,14 @@
         <v>626</v>
       </c>
       <c r="I59" s="12">
-        <f>(RIGHT(H59,LEN(H59)-4)-RIGHT(G59,LEN(G59)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J59" s="12">
         <v>240</v>
       </c>
       <c r="K59" s="91">
-        <f>I59*J59/60</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L59" s="12"/>
@@ -6353,14 +6384,14 @@
         <v>628</v>
       </c>
       <c r="I60" s="12">
-        <f>(RIGHT(H60,LEN(H60)-4)-RIGHT(G60,LEN(G60)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J60" s="12">
         <v>240</v>
       </c>
       <c r="K60" s="91">
-        <f>I60*J60/60</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L60" s="12"/>
@@ -6397,14 +6428,14 @@
         <v>630</v>
       </c>
       <c r="I61" s="12">
-        <f>(RIGHT(H61,LEN(H61)-4)-RIGHT(G61,LEN(G61)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="J61" s="12">
         <v>480</v>
       </c>
       <c r="K61" s="91">
-        <f>I61*J61/60</f>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="L61" s="12"/>
@@ -6441,14 +6472,14 @@
         <v>632</v>
       </c>
       <c r="I62" s="12">
-        <f>(RIGHT(H62,LEN(H62)-4)-RIGHT(G62,LEN(G62)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J62" s="12">
         <v>360</v>
       </c>
       <c r="K62" s="91">
-        <f>I62*J62/60</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="L62" s="12"/>
@@ -6485,14 +6516,14 @@
         <v>634</v>
       </c>
       <c r="I63" s="12">
-        <f>(RIGHT(H63,LEN(H63)-4)-RIGHT(G63,LEN(G63)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J63" s="12">
         <v>240</v>
       </c>
       <c r="K63" s="91">
-        <f>I63*J63/60</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L63" s="12"/>
@@ -6529,14 +6560,14 @@
         <v>636</v>
       </c>
       <c r="I64" s="12">
-        <f>(RIGHT(H64,LEN(H64)-4)-RIGHT(G64,LEN(G64)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J64" s="12">
         <v>300</v>
       </c>
       <c r="K64" s="91">
-        <f>I64*J64/60</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="L64" s="12"/>
@@ -6573,14 +6604,14 @@
         <v>638</v>
       </c>
       <c r="I65" s="12">
-        <f>(RIGHT(H65,LEN(H65)-4)-RIGHT(G65,LEN(G65)-4)+1)/10</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="J65" s="12">
         <v>180</v>
       </c>
       <c r="K65" s="91">
-        <f>I65*J65/60</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="L65" s="12"/>
@@ -7389,14 +7420,14 @@
         <v>491</v>
       </c>
       <c r="I86" s="16">
-        <f>(RIGHT(H86,LEN(H86)-4)-RIGHT(G86,LEN(G86)-4)+1)/10</f>
+        <f t="shared" ref="I86:I101" si="6">(RIGHT(H86,LEN(H86)-4)-RIGHT(G86,LEN(G86)-4)+1)/10</f>
         <v>10</v>
       </c>
       <c r="J86" s="16">
         <v>240</v>
       </c>
       <c r="K86" s="96">
-        <f>I86*J86/60</f>
+        <f t="shared" ref="K86:K105" si="7">I86*J86/60</f>
         <v>40</v>
       </c>
       <c r="L86" s="16"/>
@@ -7433,14 +7464,14 @@
         <v>493</v>
       </c>
       <c r="I87" s="16">
-        <f>(RIGHT(H87,LEN(H87)-4)-RIGHT(G87,LEN(G87)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J87" s="16">
         <v>480</v>
       </c>
       <c r="K87" s="96">
-        <f>I87*J87/60</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="L87" s="16"/>
@@ -7477,14 +7508,14 @@
         <v>495</v>
       </c>
       <c r="I88" s="16">
-        <f>(RIGHT(H88,LEN(H88)-4)-RIGHT(G88,LEN(G88)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="J88" s="16">
         <v>180</v>
       </c>
       <c r="K88" s="96">
-        <f>I88*J88/60</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="L88" s="16"/>
@@ -7521,14 +7552,14 @@
         <v>497</v>
       </c>
       <c r="I89" s="16">
-        <f>(RIGHT(H89,LEN(H89)-4)-RIGHT(G89,LEN(G89)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="J89" s="16">
         <v>120</v>
       </c>
       <c r="K89" s="96">
-        <f>I89*J89/60</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="L89" s="16"/>
@@ -7565,14 +7596,14 @@
         <v>499</v>
       </c>
       <c r="I90" s="16">
-        <f>(RIGHT(H90,LEN(H90)-4)-RIGHT(G90,LEN(G90)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="J90" s="16">
         <v>720</v>
       </c>
       <c r="K90" s="96">
-        <f>I90*J90/60</f>
+        <f t="shared" si="7"/>
         <v>96</v>
       </c>
       <c r="L90" s="16"/>
@@ -7609,14 +7640,14 @@
         <v>501</v>
       </c>
       <c r="I91" s="16">
-        <f>(RIGHT(H91,LEN(H91)-4)-RIGHT(G91,LEN(G91)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="J91" s="16">
         <v>300</v>
       </c>
       <c r="K91" s="96">
-        <f>I91*J91/60</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="L91" s="16"/>
@@ -7653,14 +7684,14 @@
         <v>503</v>
       </c>
       <c r="I92" s="16">
-        <f>(RIGHT(H92,LEN(H92)-4)-RIGHT(G92,LEN(G92)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="J92" s="16">
         <v>150</v>
       </c>
       <c r="K92" s="96">
-        <f>I92*J92/60</f>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
       <c r="L92" s="16"/>
@@ -7697,14 +7728,14 @@
         <v>505</v>
       </c>
       <c r="I93" s="16">
-        <f>(RIGHT(H93,LEN(H93)-4)-RIGHT(G93,LEN(G93)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="J93" s="16">
         <v>480</v>
       </c>
       <c r="K93" s="96">
-        <f>I93*J93/60</f>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="L93" s="16"/>
@@ -7741,14 +7772,14 @@
         <v>507</v>
       </c>
       <c r="I94" s="16">
-        <f>(RIGHT(H94,LEN(H94)-4)-RIGHT(G94,LEN(G94)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="J94" s="16">
         <v>600</v>
       </c>
       <c r="K94" s="96">
-        <f>I94*J94/60</f>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="L94" s="16"/>
@@ -7785,14 +7816,14 @@
         <v>509</v>
       </c>
       <c r="I95" s="16">
-        <f>(RIGHT(H95,LEN(H95)-4)-RIGHT(G95,LEN(G95)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="J95" s="16">
         <v>180</v>
       </c>
       <c r="K95" s="96">
-        <f>I95*J95/60</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="L95" s="16"/>
@@ -7829,14 +7860,14 @@
         <v>511</v>
       </c>
       <c r="I96" s="16">
-        <f>(RIGHT(H96,LEN(H96)-4)-RIGHT(G96,LEN(G96)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="J96" s="16">
         <v>360</v>
       </c>
       <c r="K96" s="96">
-        <f>I96*J96/60</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="L96" s="16"/>
@@ -7873,14 +7904,14 @@
         <v>513</v>
       </c>
       <c r="I97" s="16">
-        <f>(RIGHT(H97,LEN(H97)-4)-RIGHT(G97,LEN(G97)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J97" s="16">
         <v>360</v>
       </c>
       <c r="K97" s="96">
-        <f>I97*J97/60</f>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="L97" s="16"/>
@@ -7917,14 +7948,14 @@
         <v>515</v>
       </c>
       <c r="I98" s="16">
-        <f>(RIGHT(H98,LEN(H98)-4)-RIGHT(G98,LEN(G98)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="J98" s="16">
         <v>120</v>
       </c>
       <c r="K98" s="96">
-        <f>I98*J98/60</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="L98" s="16"/>
@@ -7961,14 +7992,14 @@
         <v>517</v>
       </c>
       <c r="I99" s="16">
-        <f>(RIGHT(H99,LEN(H99)-4)-RIGHT(G99,LEN(G99)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="J99" s="16">
         <v>360</v>
       </c>
       <c r="K99" s="96">
-        <f>I99*J99/60</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="L99" s="16"/>
@@ -8005,14 +8036,14 @@
         <v>519</v>
       </c>
       <c r="I100" s="16">
-        <f>(RIGHT(H100,LEN(H100)-4)-RIGHT(G100,LEN(G100)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J100" s="16">
         <v>120</v>
       </c>
       <c r="K100" s="96">
-        <f>I100*J100/60</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L100" s="16"/>
@@ -8049,14 +8080,14 @@
         <v>521</v>
       </c>
       <c r="I101" s="16">
-        <f>(RIGHT(H101,LEN(H101)-4)-RIGHT(G101,LEN(G101)-4)+1)/10</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="J101" s="16">
         <v>180</v>
       </c>
       <c r="K101" s="96">
-        <f>I101*J101/60</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="L101" s="16"/>
@@ -8100,7 +8131,7 @@
         <v>240</v>
       </c>
       <c r="K102" s="96">
-        <f>I102*J102/60</f>
+        <f t="shared" si="7"/>
         <v>76</v>
       </c>
       <c r="L102" s="16"/>
@@ -8144,7 +8175,7 @@
         <v>240</v>
       </c>
       <c r="K103" s="96">
-        <f>I103*J103/60</f>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="L103" s="16"/>
@@ -8188,7 +8219,7 @@
         <v>360</v>
       </c>
       <c r="K104" s="96">
-        <f>I104*J104/60</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="L104" s="16"/>
@@ -8232,7 +8263,7 @@
         <v>120</v>
       </c>
       <c r="K105" s="96">
-        <f>I105*J105/60</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="L105" s="16"/>
@@ -8652,14 +8683,14 @@
         <v>538</v>
       </c>
       <c r="I117" s="8">
-        <f>(RIGHT(H117,LEN(H117)-4)-RIGHT(G117,LEN(G117)-4)+1)/10</f>
+        <f t="shared" ref="I117:I126" si="8">(RIGHT(H117,LEN(H117)-4)-RIGHT(G117,LEN(G117)-4)+1)/10</f>
         <v>6</v>
       </c>
       <c r="J117" s="8">
         <v>240</v>
       </c>
       <c r="K117" s="66">
-        <f>I117*J117/60</f>
+        <f t="shared" ref="K117:K126" si="9">I117*J117/60</f>
         <v>24</v>
       </c>
       <c r="L117" s="8"/>
@@ -8696,14 +8727,14 @@
         <v>540</v>
       </c>
       <c r="I118" s="8">
-        <f>(RIGHT(H118,LEN(H118)-4)-RIGHT(G118,LEN(G118)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J118" s="8">
         <v>480</v>
       </c>
       <c r="K118" s="66">
-        <f>I118*J118/60</f>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="L118" s="8"/>
@@ -8740,14 +8771,14 @@
         <v>542</v>
       </c>
       <c r="I119" s="8">
-        <f>(RIGHT(H119,LEN(H119)-4)-RIGHT(G119,LEN(G119)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="J119" s="8">
         <v>480</v>
       </c>
       <c r="K119" s="66">
-        <f>I119*J119/60</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="L119" s="8"/>
@@ -8786,14 +8817,14 @@
         <v>544</v>
       </c>
       <c r="I120" s="8">
-        <f>(RIGHT(H120,LEN(H120)-4)-RIGHT(G120,LEN(G120)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="J120" s="8">
         <v>180</v>
       </c>
       <c r="K120" s="66">
-        <f>I120*J120/60</f>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="L120" s="8"/>
@@ -8830,14 +8861,14 @@
         <v>546</v>
       </c>
       <c r="I121" s="8">
-        <f>(RIGHT(H121,LEN(H121)-4)-RIGHT(G121,LEN(G121)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J121" s="8">
         <v>150</v>
       </c>
       <c r="K121" s="66">
-        <f>I121*J121/60</f>
+        <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
       <c r="L121" s="8"/>
@@ -8874,14 +8905,14 @@
         <v>548</v>
       </c>
       <c r="I122" s="8">
-        <f>(RIGHT(H122,LEN(H122)-4)-RIGHT(G122,LEN(G122)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J122" s="8">
         <v>150</v>
       </c>
       <c r="K122" s="66">
-        <f>I122*J122/60</f>
+        <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
       <c r="L122" s="8"/>
@@ -8918,14 +8949,14 @@
         <v>550</v>
       </c>
       <c r="I123" s="8">
-        <f>(RIGHT(H123,LEN(H123)-4)-RIGHT(G123,LEN(G123)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J123" s="8">
         <v>150</v>
       </c>
       <c r="K123" s="66">
-        <f>I123*J123/60</f>
+        <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
       <c r="L123" s="8"/>
@@ -8962,14 +8993,14 @@
         <v>552</v>
       </c>
       <c r="I124" s="8">
-        <f>(RIGHT(H124,LEN(H124)-4)-RIGHT(G124,LEN(G124)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J124" s="8">
         <v>150</v>
       </c>
       <c r="K124" s="66">
-        <f>I124*J124/60</f>
+        <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
       <c r="L124" s="8"/>
@@ -9006,14 +9037,14 @@
         <v>554</v>
       </c>
       <c r="I125" s="8">
-        <f>(RIGHT(H125,LEN(H125)-4)-RIGHT(G125,LEN(G125)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="J125" s="8">
         <v>360</v>
       </c>
       <c r="K125" s="66">
-        <f>I125*J125/60</f>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="L125" s="8"/>
@@ -9050,14 +9081,14 @@
         <v>556</v>
       </c>
       <c r="I126" s="8">
-        <f>(RIGHT(H126,LEN(H126)-4)-RIGHT(G126,LEN(G126)-4)+1)/10</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="J126" s="8">
         <v>240</v>
       </c>
       <c r="K126" s="66">
-        <f>I126*J126/60</f>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="L126" s="8"/>
@@ -9127,7 +9158,7 @@
         <v>420</v>
       </c>
       <c r="K128" s="60">
-        <f>I128*J128/60</f>
+        <f t="shared" ref="K128:K135" si="10">I128*J128/60</f>
         <v>70</v>
       </c>
       <c r="L128" s="10" t="s">
@@ -9179,7 +9210,7 @@
         <v>180</v>
       </c>
       <c r="K129" s="60">
-        <f>I129*J129/60</f>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
       <c r="L129" s="10" t="s">
@@ -9220,14 +9251,14 @@
         <v>463</v>
       </c>
       <c r="I130" s="10">
-        <f>(RIGHT(H130,LEN(H130)-4)-RIGHT(G130,LEN(G130)-4)+1)/10</f>
+        <f t="shared" ref="I130:I135" si="11">(RIGHT(H130,LEN(H130)-4)-RIGHT(G130,LEN(G130)-4)+1)/10</f>
         <v>8</v>
       </c>
       <c r="J130" s="10">
         <v>180</v>
       </c>
       <c r="K130" s="60">
-        <f>I130*J130/60</f>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="L130" s="10"/>
@@ -9270,14 +9301,14 @@
         <v>465</v>
       </c>
       <c r="I131" s="10">
-        <f>(RIGHT(H131,LEN(H131)-4)-RIGHT(G131,LEN(G131)-4)+1)/10</f>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="J131" s="10">
         <v>180</v>
       </c>
       <c r="K131" s="60">
-        <f>I131*J131/60</f>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
       <c r="L131" s="10"/>
@@ -9316,14 +9347,14 @@
         <v>467</v>
       </c>
       <c r="I132" s="10">
-        <f>(RIGHT(H132,LEN(H132)-4)-RIGHT(G132,LEN(G132)-4)+1)/10</f>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="J132" s="10">
         <v>90</v>
       </c>
       <c r="K132" s="60">
-        <f>I132*J132/60</f>
+        <f t="shared" si="10"/>
         <v>22.5</v>
       </c>
       <c r="L132" s="10"/>
@@ -9366,14 +9397,14 @@
         <v>470</v>
       </c>
       <c r="I133" s="10">
-        <f>(RIGHT(H133,LEN(H133)-4)-RIGHT(G133,LEN(G133)-4)+1)/10</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="J133" s="10">
         <v>150</v>
       </c>
       <c r="K133" s="60">
-        <f>I133*J133/60</f>
+        <f t="shared" si="10"/>
         <v>12.5</v>
       </c>
       <c r="L133" s="10" t="s">
@@ -9414,14 +9445,14 @@
         <v>472</v>
       </c>
       <c r="I134" s="10">
-        <f>(RIGHT(H134,LEN(H134)-4)-RIGHT(G134,LEN(G134)-4)+1)/10</f>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="J134" s="10">
         <v>240</v>
       </c>
       <c r="K134" s="60">
-        <f>I134*J134/60</f>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="L134" s="10" t="s">
@@ -9466,14 +9497,14 @@
         <v>474</v>
       </c>
       <c r="I135" s="10">
-        <f>(RIGHT(H135,LEN(H135)-4)-RIGHT(G135,LEN(G135)-4)+1)/10</f>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="J135" s="10">
         <v>240</v>
       </c>
       <c r="K135" s="60">
-        <f>I135*J135/60</f>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
       <c r="L135" s="10" t="s">
@@ -9844,8 +9875,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>